<commit_message>
MHDV and Supplementary Code Path Update
</commit_message>
<xml_diff>
--- a/input/rail_aviation_ship_county_share.xlsx
+++ b/input/rail_aviation_ship_county_share.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_3073\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/samrat_acharya_pnnl_gov/Documents/Documents/GOODEEP/transportation_electrification/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1599B24-EB66-4A78-99FB-0AC775C96A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{E1599B24-EB66-4A78-99FB-0AC775C96A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE78C2FE-DEE8-4083-82C5-85AEC9BE3C3B}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -1359,7 +1359,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2196,11 +2196,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N508"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2244,7 +2251,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4001</v>
       </c>
@@ -2270,7 +2277,7 @@
         <v>6.0712267E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4003</v>
       </c>
@@ -2296,7 +2303,7 @@
         <v>0.114867157</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4005</v>
       </c>
@@ -2331,7 +2338,7 @@
         <v>6.0924109999999998E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4007</v>
       </c>
@@ -2357,7 +2364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4009</v>
       </c>
@@ -2383,7 +2390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4011</v>
       </c>
@@ -2409,7 +2416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4012</v>
       </c>
@@ -2435,7 +2442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4013</v>
       </c>
@@ -2470,7 +2477,7 @@
         <v>0.92536299099999997</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4015</v>
       </c>
@@ -2496,7 +2503,7 @@
         <v>0.135104579</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4017</v>
       </c>
@@ -2531,7 +2538,7 @@
         <v>2.14277E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4019</v>
       </c>
@@ -2566,7 +2573,7 @@
         <v>6.2057672000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4021</v>
       </c>
@@ -2592,7 +2599,7 @@
         <v>7.8349349999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4023</v>
       </c>
@@ -2618,7 +2625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4025</v>
       </c>
@@ -2653,7 +2660,7 @@
         <v>1.1064580000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4027</v>
       </c>
@@ -2688,7 +2695,7 @@
         <v>5.1661900000000002E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6001</v>
       </c>
@@ -2732,7 +2739,7 @@
         <v>7.1065989999999996E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6003</v>
       </c>
@@ -2758,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6005</v>
       </c>
@@ -2790,7 +2797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6007</v>
       </c>
@@ -2822,7 +2829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6009</v>
       </c>
@@ -2848,7 +2855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6011</v>
       </c>
@@ -2880,7 +2887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6013</v>
       </c>
@@ -2915,7 +2922,7 @@
         <v>9.6446700999999996E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6015</v>
       </c>
@@ -2953,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6017</v>
       </c>
@@ -2979,7 +2986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6019</v>
       </c>
@@ -3020,7 +3027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>6021</v>
       </c>
@@ -3052,7 +3059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6023</v>
       </c>
@@ -3090,7 +3097,7 @@
         <v>5.0761419999999996E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6025</v>
       </c>
@@ -3131,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6027</v>
       </c>
@@ -3157,7 +3164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6029</v>
       </c>
@@ -3198,7 +3205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6031</v>
       </c>
@@ -3230,7 +3237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>6033</v>
       </c>
@@ -3256,7 +3263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>6035</v>
       </c>
@@ -3288,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>6037</v>
       </c>
@@ -3332,7 +3339,7 @@
         <v>0.49238578700000002</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>6039</v>
       </c>
@@ -3364,7 +3371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>6041</v>
       </c>
@@ -3399,7 +3406,7 @@
         <v>5.0761419999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>6043</v>
       </c>
@@ -3425,7 +3432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>6045</v>
       </c>
@@ -3460,7 +3467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>6047</v>
       </c>
@@ -3501,7 +3508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>6049</v>
       </c>
@@ -3533,7 +3540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6051</v>
       </c>
@@ -3559,7 +3566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>6053</v>
       </c>
@@ -3603,7 +3610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>6055</v>
       </c>
@@ -3635,7 +3642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>6057</v>
       </c>
@@ -3667,7 +3674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>6059</v>
       </c>
@@ -3711,7 +3718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>6061</v>
       </c>
@@ -3743,7 +3750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>6063</v>
       </c>
@@ -3775,7 +3782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>6065</v>
       </c>
@@ -3816,7 +3823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>6067</v>
       </c>
@@ -3860,7 +3867,7 @@
         <v>1.0152283999999999E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>6069</v>
       </c>
@@ -3892,7 +3899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>6071</v>
       </c>
@@ -3933,7 +3940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>6073</v>
       </c>
@@ -3977,7 +3984,7 @@
         <v>0.10659898499999999</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>6075</v>
       </c>
@@ -4012,7 +4019,7 @@
         <v>0.101522843</v>
       </c>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>6077</v>
       </c>
@@ -4056,7 +4063,7 @@
         <v>1.0152283999999999E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>6079</v>
       </c>
@@ -4100,7 +4107,7 @@
         <v>5.0761419999999996E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>6081</v>
       </c>
@@ -4144,7 +4151,7 @@
         <v>2.5380711E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>6083</v>
       </c>
@@ -4188,7 +4195,7 @@
         <v>5.0761419999999996E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>6085</v>
       </c>
@@ -4229,7 +4236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>6087</v>
       </c>
@@ -4261,7 +4268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>6089</v>
       </c>
@@ -4302,7 +4309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>6091</v>
       </c>
@@ -4334,7 +4341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>6093</v>
       </c>
@@ -4366,7 +4373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>6095</v>
       </c>
@@ -4401,7 +4408,7 @@
         <v>2.0304569000000001E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:14">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>6097</v>
       </c>
@@ -4445,7 +4452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>6099</v>
       </c>
@@ -4477,7 +4484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>6101</v>
       </c>
@@ -4509,7 +4516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>6103</v>
       </c>
@@ -4541,7 +4548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>6105</v>
       </c>
@@ -4567,7 +4574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>6107</v>
       </c>
@@ -4599,7 +4606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>6109</v>
       </c>
@@ -4631,7 +4638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>6111</v>
       </c>
@@ -4666,7 +4673,7 @@
         <v>4.5685279000000002E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>6113</v>
       </c>
@@ -4701,7 +4708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>6115</v>
       </c>
@@ -4733,7 +4740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>8001</v>
       </c>
@@ -4759,7 +4766,7 @@
         <v>3.2520325000000003E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>8003</v>
       </c>
@@ -4794,7 +4801,7 @@
         <v>3.8783399999999999E-4</v>
       </c>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>8005</v>
       </c>
@@ -4820,7 +4827,7 @@
         <v>5.1619559999999997E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>8007</v>
       </c>
@@ -4846,7 +4853,7 @@
         <v>2.1938309999999998E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>8009</v>
       </c>
@@ -4872,7 +4879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:14">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>8011</v>
       </c>
@@ -4898,7 +4905,7 @@
         <v>4.7619047999999997E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>8013</v>
       </c>
@@ -4924,7 +4931,7 @@
         <v>1.1356303999999999E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>8014</v>
       </c>
@@ -4950,7 +4957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>8015</v>
       </c>
@@ -4970,7 +4977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>8017</v>
       </c>
@@ -4996,7 +5003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>8019</v>
       </c>
@@ -5016,7 +5023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>8021</v>
       </c>
@@ -5042,7 +5049,7 @@
         <v>4.2457091000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>8023</v>
       </c>
@@ -5068,7 +5075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>8025</v>
       </c>
@@ -5088,7 +5095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>8027</v>
       </c>
@@ -5108,7 +5115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>8029</v>
       </c>
@@ -5134,7 +5141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>8031</v>
       </c>
@@ -5169,7 +5176,7 @@
         <v>0.92681364399999999</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>8033</v>
       </c>
@@ -5189,7 +5196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>8035</v>
       </c>
@@ -5215,7 +5222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>8037</v>
       </c>
@@ -5250,7 +5257,7 @@
         <v>6.5275990000000002E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>8039</v>
       </c>
@@ -5276,7 +5283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>8041</v>
       </c>
@@ -5311,7 +5318,7 @@
         <v>3.0475316999999998E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>8043</v>
       </c>
@@ -5337,7 +5344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>8045</v>
       </c>
@@ -5363,7 +5370,7 @@
         <v>8.4010840000000003E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>8047</v>
       </c>
@@ -5389,7 +5396,7 @@
         <v>2.1680217000000002E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>8049</v>
       </c>
@@ -5415,7 +5422,7 @@
         <v>8.4527036E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>8051</v>
       </c>
@@ -5450,7 +5457,7 @@
         <v>1.2548069999999999E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:11">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>8053</v>
       </c>
@@ -5470,7 +5477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>8055</v>
       </c>
@@ -5496,7 +5503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:11">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>8057</v>
       </c>
@@ -5516,7 +5523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>8059</v>
       </c>
@@ -5542,7 +5549,7 @@
         <v>3.3294618999999998E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:11">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>8061</v>
       </c>
@@ -5568,7 +5575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:11">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>8063</v>
       </c>
@@ -5594,7 +5601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:11">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>8065</v>
       </c>
@@ -5614,7 +5621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:11">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>8067</v>
       </c>
@@ -5649,7 +5656,7 @@
         <v>6.4788399999999996E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:11">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>8069</v>
       </c>
@@ -5684,7 +5691,7 @@
         <v>1.6979699999999999E-4</v>
       </c>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>8071</v>
       </c>
@@ -5710,7 +5717,7 @@
         <v>7.8332687999999998E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>8073</v>
       </c>
@@ -5736,7 +5743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:11">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>8075</v>
       </c>
@@ -5762,7 +5769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:11">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>8077</v>
       </c>
@@ -5797,7 +5804,7 @@
         <v>8.1627339999999996E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:11">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>8079</v>
       </c>
@@ -5817,7 +5824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:11">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>8081</v>
       </c>
@@ -5843,7 +5850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:11">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>8083</v>
       </c>
@@ -5872,7 +5879,7 @@
         <v>2.0043700000000001E-4</v>
       </c>
     </row>
-    <row r="118" spans="1:11">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>8085</v>
       </c>
@@ -5907,7 +5914,7 @@
         <v>6.0941449999999996E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:11">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>8087</v>
       </c>
@@ -5933,7 +5940,7 @@
         <v>4.8135243000000001E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:11">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>8089</v>
       </c>
@@ -5959,7 +5966,7 @@
         <v>5.7942960000000002E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:11">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>8091</v>
       </c>
@@ -5979,7 +5986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:11">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>8093</v>
       </c>
@@ -5999,7 +6006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:11">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>8095</v>
       </c>
@@ -6025,7 +6032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:11">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>8097</v>
       </c>
@@ -6054,7 +6061,7 @@
         <v>8.0492020000000001E-3</v>
       </c>
     </row>
-    <row r="125" spans="1:11">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>8099</v>
       </c>
@@ -6080,7 +6087,7 @@
         <v>4.9296683000000001E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:11">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>8101</v>
       </c>
@@ -6115,7 +6122,7 @@
         <v>3.1137999999999999E-4</v>
       </c>
     </row>
-    <row r="127" spans="1:11">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>8103</v>
       </c>
@@ -6141,7 +6148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:11">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>8105</v>
       </c>
@@ -6167,7 +6174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:11">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>8107</v>
       </c>
@@ -6202,7 +6209,7 @@
         <v>4.8577799999999999E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:11">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>8109</v>
       </c>
@@ -6228,7 +6235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:11">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>8111</v>
       </c>
@@ -6254,7 +6261,7 @@
         <v>1.7292554000000002E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:11">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>8113</v>
       </c>
@@ -6283,7 +6290,7 @@
         <v>2.16484E-4</v>
       </c>
     </row>
-    <row r="133" spans="1:11">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>8115</v>
       </c>
@@ -6309,7 +6316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:11">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>8117</v>
       </c>
@@ -6329,7 +6336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:11">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>8119</v>
       </c>
@@ -6349,7 +6356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:11">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>8121</v>
       </c>
@@ -6375,7 +6382,7 @@
         <v>4.8264292E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:11">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>8123</v>
       </c>
@@ -6401,7 +6408,7 @@
         <v>4.5812363000000002E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:11">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>8125</v>
       </c>
@@ -6427,7 +6434,7 @@
         <v>5.1748612999999999E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:11">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>16001</v>
       </c>
@@ -6462,7 +6469,7 @@
         <v>0.81829358900000004</v>
       </c>
     </row>
-    <row r="140" spans="1:11">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>16003</v>
       </c>
@@ -6482,7 +6489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:11">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>16005</v>
       </c>
@@ -6508,7 +6515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:11">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>16007</v>
       </c>
@@ -6534,7 +6541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:11">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>16009</v>
       </c>
@@ -6560,7 +6567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:11">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>16011</v>
       </c>
@@ -6586,7 +6593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:11">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>16013</v>
       </c>
@@ -6621,7 +6628,7 @@
         <v>4.2595596999999999E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:11">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>16015</v>
       </c>
@@ -6647,7 +6654,7 @@
         <v>0.18382352900000001</v>
       </c>
     </row>
-    <row r="147" spans="1:11">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>16017</v>
       </c>
@@ -6673,7 +6680,7 @@
         <v>0.27740641700000002</v>
       </c>
     </row>
-    <row r="148" spans="1:11">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>16019</v>
       </c>
@@ -6708,7 +6715,7 @@
         <v>9.8549417E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:11">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>16021</v>
       </c>
@@ -6734,7 +6741,7 @@
         <v>0.23128342199999999</v>
       </c>
     </row>
-    <row r="150" spans="1:11">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>16023</v>
       </c>
@@ -6760,7 +6767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:11">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>16025</v>
       </c>
@@ -6780,7 +6787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:11">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>16027</v>
       </c>
@@ -6806,7 +6813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:11">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>16029</v>
       </c>
@@ -6832,7 +6839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:11">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>16031</v>
       </c>
@@ -6858,7 +6865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:11">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>16033</v>
       </c>
@@ -6884,7 +6891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:11">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>16035</v>
       </c>
@@ -6910,7 +6917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:11">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>16037</v>
       </c>
@@ -6930,7 +6937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:11">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>16039</v>
       </c>
@@ -6956,7 +6963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:11">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>16041</v>
       </c>
@@ -6982,7 +6989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:11">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>16043</v>
       </c>
@@ -7008,7 +7015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:11">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>16045</v>
       </c>
@@ -7034,7 +7041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:11">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>16047</v>
       </c>
@@ -7060,7 +7067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:11">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>16049</v>
       </c>
@@ -7086,7 +7093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:11">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>16051</v>
       </c>
@@ -7112,7 +7119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:11">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>16053</v>
       </c>
@@ -7138,7 +7145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:11">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>16055</v>
       </c>
@@ -7164,7 +7171,7 @@
         <v>0.15975935799999999</v>
       </c>
     </row>
-    <row r="167" spans="1:11">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>16057</v>
       </c>
@@ -7190,7 +7197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:11">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>16059</v>
       </c>
@@ -7210,7 +7217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:11">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>16061</v>
       </c>
@@ -7236,7 +7243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:11">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>16063</v>
       </c>
@@ -7262,7 +7269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:11">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>16065</v>
       </c>
@@ -7288,7 +7295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:11">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>16067</v>
       </c>
@@ -7314,7 +7321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:11">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>16069</v>
       </c>
@@ -7349,7 +7356,7 @@
         <v>1.3973866999999999E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:11">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>16071</v>
       </c>
@@ -7375,7 +7382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:11">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>16073</v>
       </c>
@@ -7395,7 +7402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:11">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>16075</v>
       </c>
@@ -7421,7 +7428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:11">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>16077</v>
       </c>
@@ -7456,7 +7463,7 @@
         <v>1.0773972999999999E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:11">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>16079</v>
       </c>
@@ -7476,7 +7483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:11">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>16081</v>
       </c>
@@ -7496,7 +7503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:11">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>16083</v>
       </c>
@@ -7531,7 +7538,7 @@
         <v>1.5813557999999998E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:11">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>16085</v>
       </c>
@@ -7557,7 +7564,7 @@
         <v>0.14772727299999999</v>
       </c>
     </row>
-    <row r="182" spans="1:11">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>16087</v>
       </c>
@@ -7583,7 +7590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:11">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>30001</v>
       </c>
@@ -7609,7 +7616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:11">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>30003</v>
       </c>
@@ -7635,7 +7642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:11">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>30005</v>
       </c>
@@ -7661,7 +7668,7 @@
         <v>7.9453225000000002E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:11">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>30007</v>
       </c>
@@ -7687,7 +7694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:11">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>30009</v>
       </c>
@@ -7713,7 +7720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:11">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>30011</v>
       </c>
@@ -7733,7 +7740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:11">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>30013</v>
       </c>
@@ -7768,7 +7775,7 @@
         <v>5.4923549000000002E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:11">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>30015</v>
       </c>
@@ -7794,7 +7801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:11">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>30017</v>
       </c>
@@ -7820,7 +7827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:11">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>30019</v>
       </c>
@@ -7846,7 +7853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:11">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>30021</v>
       </c>
@@ -7872,7 +7879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:11">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>30023</v>
       </c>
@@ -7898,7 +7905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:11">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>30025</v>
       </c>
@@ -7924,7 +7931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:11">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>30027</v>
       </c>
@@ -7950,7 +7957,7 @@
         <v>3.5882101999999999E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:11">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>30029</v>
       </c>
@@ -7985,7 +7992,7 @@
         <v>0.173612513</v>
       </c>
     </row>
-    <row r="198" spans="1:11">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>30031</v>
       </c>
@@ -8020,7 +8027,7 @@
         <v>0.40979286599999998</v>
       </c>
     </row>
-    <row r="199" spans="1:11">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>30033</v>
       </c>
@@ -8040,7 +8047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:11">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>30035</v>
       </c>
@@ -8066,7 +8073,7 @@
         <v>9.4973658000000002E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:11">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>30037</v>
       </c>
@@ -8092,7 +8099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:11">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>30039</v>
       </c>
@@ -8118,7 +8125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:11">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>30041</v>
       </c>
@@ -8153,7 +8160,7 @@
         <v>1.4097650000000001E-3</v>
       </c>
     </row>
-    <row r="204" spans="1:11">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>30043</v>
       </c>
@@ -8179,7 +8186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:11">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>30045</v>
       </c>
@@ -8205,7 +8212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:11">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>30047</v>
       </c>
@@ -8231,7 +8238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:11">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>30049</v>
       </c>
@@ -8266,7 +8273,7 @@
         <v>2.9609226999999998E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:11">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>30051</v>
       </c>
@@ -8292,7 +8299,7 @@
         <v>3.7305995000000002E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:11">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>30053</v>
       </c>
@@ -8318,7 +8325,7 @@
         <v>0.14865442100000001</v>
       </c>
     </row>
-    <row r="210" spans="1:11">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>30055</v>
       </c>
@@ -8344,7 +8351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:11">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>30057</v>
       </c>
@@ -8370,7 +8377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:11">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>30059</v>
       </c>
@@ -8390,7 +8397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:11">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>30061</v>
       </c>
@@ -8416,7 +8423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:11">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>30063</v>
       </c>
@@ -8451,7 +8458,7 @@
         <v>0.159839166</v>
       </c>
     </row>
-    <row r="215" spans="1:11">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>30065</v>
       </c>
@@ -8477,7 +8484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:11">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>30067</v>
       </c>
@@ -8503,7 +8510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:11">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>30069</v>
       </c>
@@ -8523,7 +8530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:11">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>30071</v>
       </c>
@@ -8549,7 +8556,7 @@
         <v>7.4896768000000002E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:11">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>30073</v>
       </c>
@@ -8575,7 +8582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:11">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>30075</v>
       </c>
@@ -8595,7 +8602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:11">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>30077</v>
       </c>
@@ -8621,7 +8628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:11">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>30079</v>
       </c>
@@ -8647,7 +8654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:11">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>30081</v>
       </c>
@@ -8667,7 +8674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:11">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>30083</v>
       </c>
@@ -8702,7 +8709,7 @@
         <v>3.4698089999999999E-3</v>
       </c>
     </row>
-    <row r="225" spans="1:11">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>30085</v>
       </c>
@@ -8737,7 +8744,7 @@
         <v>1.4953060000000001E-3</v>
       </c>
     </row>
-    <row r="226" spans="1:11">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>30087</v>
       </c>
@@ -8763,7 +8770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:11">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>30089</v>
       </c>
@@ -8789,7 +8796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:11">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>30091</v>
       </c>
@@ -8815,7 +8822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:11">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>30093</v>
       </c>
@@ -8850,7 +8857,7 @@
         <v>6.9375410000000002E-3</v>
       </c>
     </row>
-    <row r="230" spans="1:11">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>30095</v>
       </c>
@@ -8876,7 +8883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:11">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>30097</v>
       </c>
@@ -8902,7 +8909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:11">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>30099</v>
       </c>
@@ -8928,7 +8935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:11">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>30101</v>
       </c>
@@ -8954,7 +8961,7 @@
         <v>6.3790402999999996E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:11">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>30103</v>
       </c>
@@ -8980,7 +8987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:11">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>30105</v>
       </c>
@@ -9015,7 +9022,7 @@
         <v>1.4068590000000001E-3</v>
       </c>
     </row>
-    <row r="236" spans="1:11">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>30107</v>
       </c>
@@ -9041,7 +9048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:11">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>30109</v>
       </c>
@@ -9067,7 +9074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:11">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>30111</v>
       </c>
@@ -9102,7 +9109,7 @@
         <v>0.15750339899999999</v>
       </c>
     </row>
-    <row r="239" spans="1:11">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>31001</v>
       </c>
@@ -9128,7 +9135,7 @@
         <v>6.0568295000000001E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:11">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>31003</v>
       </c>
@@ -9154,7 +9161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:8">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>31005</v>
       </c>
@@ -9174,7 +9181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:8">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>31007</v>
       </c>
@@ -9194,7 +9201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:8">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>31009</v>
       </c>
@@ -9220,7 +9227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:8">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>31011</v>
       </c>
@@ -9246,7 +9253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:8">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>31013</v>
       </c>
@@ -9272,7 +9279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:8">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>31015</v>
       </c>
@@ -9292,7 +9299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:8">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>31017</v>
       </c>
@@ -9312,7 +9319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:8">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>31019</v>
       </c>
@@ -9338,7 +9345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:8">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>31021</v>
       </c>
@@ -9364,7 +9371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:8">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>31023</v>
       </c>
@@ -9390,7 +9397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:8">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>31025</v>
       </c>
@@ -9416,7 +9423,7 @@
         <v>3.0408774E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:8">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>31027</v>
       </c>
@@ -9442,7 +9449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:8">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>31029</v>
       </c>
@@ -9468,7 +9475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:8">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>31031</v>
       </c>
@@ -9488,7 +9495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:8">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>31033</v>
       </c>
@@ -9514,7 +9521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:8">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>31035</v>
       </c>
@@ -9540,7 +9547,7 @@
         <v>6.1316052000000003E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:8">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>31037</v>
       </c>
@@ -9566,7 +9573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:8">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>31039</v>
       </c>
@@ -9586,7 +9593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:8">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>31041</v>
       </c>
@@ -9612,7 +9619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:8">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>31043</v>
       </c>
@@ -9638,7 +9645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:8">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>31045</v>
       </c>
@@ -9664,7 +9671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:8">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>31047</v>
       </c>
@@ -9690,7 +9697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:8">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>31049</v>
       </c>
@@ -9716,7 +9723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:8">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>31051</v>
       </c>
@@ -9742,7 +9749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:8">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>31053</v>
       </c>
@@ -9768,7 +9775,7 @@
         <v>4.0378863000000001E-2</v>
       </c>
     </row>
-    <row r="266" spans="1:8">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>31055</v>
       </c>
@@ -9794,7 +9801,7 @@
         <v>3.5393819E-2</v>
       </c>
     </row>
-    <row r="267" spans="1:8">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>31057</v>
       </c>
@@ -9820,7 +9827,7 @@
         <v>0.102941176</v>
       </c>
     </row>
-    <row r="268" spans="1:8">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>31059</v>
       </c>
@@ -9846,7 +9853,7 @@
         <v>5.9322034000000003E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:8">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>31061</v>
       </c>
@@ -9872,7 +9879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:8">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>31063</v>
       </c>
@@ -9898,7 +9905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:8">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>31065</v>
       </c>
@@ -9924,7 +9931,7 @@
         <v>7.6021933999999999E-2</v>
       </c>
     </row>
-    <row r="272" spans="1:8">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>31067</v>
       </c>
@@ -9950,7 +9957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:8">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>31069</v>
       </c>
@@ -9976,7 +9983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:8">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>31071</v>
       </c>
@@ -9996,7 +10003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:8">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>31073</v>
       </c>
@@ -10022,7 +10029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:8">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>31075</v>
       </c>
@@ -10048,7 +10055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:8">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>31077</v>
       </c>
@@ -10074,7 +10081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:8">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>31079</v>
       </c>
@@ -10100,7 +10107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:8">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>31081</v>
       </c>
@@ -10126,7 +10133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:8">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>31083</v>
       </c>
@@ -10152,7 +10159,7 @@
         <v>3.4895313999999997E-2</v>
       </c>
     </row>
-    <row r="281" spans="1:8">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>31085</v>
       </c>
@@ -10178,7 +10185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:8">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>31087</v>
       </c>
@@ -10204,7 +10211,7 @@
         <v>7.7018943000000006E-2</v>
       </c>
     </row>
-    <row r="283" spans="1:8">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>31089</v>
       </c>
@@ -10230,7 +10237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:8">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>31091</v>
       </c>
@@ -10256,7 +10263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:8">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>31093</v>
       </c>
@@ -10282,7 +10289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:8">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>31095</v>
       </c>
@@ -10308,7 +10315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:8">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>31097</v>
       </c>
@@ -10334,7 +10341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:8">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>31099</v>
       </c>
@@ -10360,7 +10367,7 @@
         <v>6.4057826999999998E-2</v>
       </c>
     </row>
-    <row r="289" spans="1:8">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>31101</v>
       </c>
@@ -10386,7 +10393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:8">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>31103</v>
       </c>
@@ -10406,7 +10413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:8">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>31105</v>
       </c>
@@ -10432,7 +10439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:8">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>31107</v>
       </c>
@@ -10452,7 +10459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:8">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>31109</v>
       </c>
@@ -10478,7 +10485,7 @@
         <v>8.3998006E-2</v>
       </c>
     </row>
-    <row r="294" spans="1:8">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>31111</v>
       </c>
@@ -10504,7 +10511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:8">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>31113</v>
       </c>
@@ -10524,7 +10531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:8">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>31115</v>
       </c>
@@ -10544,7 +10551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:8">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>31117</v>
       </c>
@@ -10564,7 +10571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:8">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>31119</v>
       </c>
@@ -10590,7 +10597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:8">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>31121</v>
       </c>
@@ -10616,7 +10623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:8">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>31123</v>
       </c>
@@ -10642,7 +10649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:8">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>31125</v>
       </c>
@@ -10668,7 +10675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:8">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>31127</v>
       </c>
@@ -10694,7 +10701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:8">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>31129</v>
       </c>
@@ -10720,7 +10727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:8">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>31131</v>
       </c>
@@ -10746,7 +10753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:8">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>31133</v>
       </c>
@@ -10772,7 +10779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:8">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>31135</v>
       </c>
@@ -10798,7 +10805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:8">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>31137</v>
       </c>
@@ -10824,7 +10831,7 @@
         <v>4.7607178E-2</v>
       </c>
     </row>
-    <row r="308" spans="1:8">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>31139</v>
       </c>
@@ -10850,7 +10857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:8">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>31141</v>
       </c>
@@ -10876,7 +10883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:8">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>31143</v>
       </c>
@@ -10902,7 +10909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:8">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>31145</v>
       </c>
@@ -10928,7 +10935,7 @@
         <v>7.7018943000000006E-2</v>
       </c>
     </row>
-    <row r="312" spans="1:8">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>31147</v>
       </c>
@@ -10954,7 +10961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:8">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>31149</v>
       </c>
@@ -10974,7 +10981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:8">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>31151</v>
       </c>
@@ -11000,7 +11007,7 @@
         <v>6.2562312999999994E-2</v>
       </c>
     </row>
-    <row r="315" spans="1:8">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>31153</v>
       </c>
@@ -11026,7 +11033,7 @@
         <v>7.5024925000000006E-2</v>
       </c>
     </row>
-    <row r="316" spans="1:8">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>31155</v>
       </c>
@@ -11052,7 +11059,7 @@
         <v>1.1465603E-2</v>
       </c>
     </row>
-    <row r="317" spans="1:8">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>31157</v>
       </c>
@@ -11078,7 +11085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:8">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>31159</v>
       </c>
@@ -11104,7 +11111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:8">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>31161</v>
       </c>
@@ -11130,7 +11137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:8">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>31163</v>
       </c>
@@ -11156,7 +11163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:11">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>31165</v>
       </c>
@@ -11182,7 +11189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:11">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>31167</v>
       </c>
@@ -11202,7 +11209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:11">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>31169</v>
       </c>
@@ -11228,7 +11235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:11">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>31171</v>
       </c>
@@ -11254,7 +11261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:11">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>31173</v>
       </c>
@@ -11280,7 +11287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:11">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>31175</v>
       </c>
@@ -11306,7 +11313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:11">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>31177</v>
       </c>
@@ -11332,7 +11339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:11">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>31179</v>
       </c>
@@ -11352,7 +11359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:11">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>31181</v>
       </c>
@@ -11378,7 +11385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:11">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>31183</v>
       </c>
@@ -11398,7 +11405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:11">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>31185</v>
       </c>
@@ -11424,7 +11431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:11">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>32001</v>
       </c>
@@ -11450,7 +11457,7 @@
         <v>6.0781476000000001E-2</v>
       </c>
     </row>
-    <row r="333" spans="1:11">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>32003</v>
       </c>
@@ -11485,7 +11492,7 @@
         <v>0.91435017399999996</v>
       </c>
     </row>
-    <row r="334" spans="1:11">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>32005</v>
       </c>
@@ -11505,7 +11512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:11">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>32007</v>
       </c>
@@ -11540,7 +11547,7 @@
         <v>7.4531499999999997E-4</v>
       </c>
     </row>
-    <row r="336" spans="1:11">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>32009</v>
       </c>
@@ -11560,7 +11567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:11">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>32011</v>
       </c>
@@ -11586,7 +11593,7 @@
         <v>9.7684515E-2</v>
       </c>
     </row>
-    <row r="338" spans="1:11">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>32013</v>
       </c>
@@ -11612,7 +11619,7 @@
         <v>0.162228654</v>
       </c>
     </row>
-    <row r="339" spans="1:11">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>32015</v>
       </c>
@@ -11638,7 +11645,7 @@
         <v>7.5253256000000004E-2</v>
       </c>
     </row>
-    <row r="340" spans="1:11">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>32017</v>
       </c>
@@ -11664,7 +11671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:11">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>32019</v>
       </c>
@@ -11690,7 +11697,7 @@
         <v>1.5774239999999998E-2</v>
       </c>
     </row>
-    <row r="342" spans="1:11">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>32021</v>
       </c>
@@ -11716,7 +11723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:11">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>32023</v>
       </c>
@@ -11736,7 +11743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:11">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>32027</v>
       </c>
@@ -11762,7 +11769,7 @@
         <v>0.108972504</v>
       </c>
     </row>
-    <row r="345" spans="1:11">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>32029</v>
       </c>
@@ -11788,7 +11795,7 @@
         <v>1.4761216000000001E-2</v>
       </c>
     </row>
-    <row r="346" spans="1:11">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>32031</v>
       </c>
@@ -11823,7 +11830,7 @@
         <v>8.4904510000000002E-2</v>
       </c>
     </row>
-    <row r="347" spans="1:11">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>32033</v>
       </c>
@@ -11849,7 +11856,7 @@
         <v>4.6164978000000002E-2</v>
       </c>
     </row>
-    <row r="348" spans="1:11">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>32510</v>
       </c>
@@ -11869,7 +11876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:11">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>35001</v>
       </c>
@@ -11904,7 +11911,7 @@
         <v>0.90910050200000003</v>
       </c>
     </row>
-    <row r="350" spans="1:11">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>35003</v>
       </c>
@@ -11924,7 +11931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:11">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>35005</v>
       </c>
@@ -11959,7 +11966,7 @@
         <v>2.4161085999999998E-2</v>
       </c>
     </row>
-    <row r="352" spans="1:11">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>35006</v>
       </c>
@@ -11985,7 +11992,7 @@
         <v>8.3806818000000005E-2</v>
       </c>
     </row>
-    <row r="353" spans="1:11">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>35007</v>
       </c>
@@ -12011,7 +12018,7 @@
         <v>8.3096590999999997E-2</v>
       </c>
     </row>
-    <row r="354" spans="1:11">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>35009</v>
       </c>
@@ -12046,7 +12053,7 @@
         <v>4.0780820000000002E-3</v>
       </c>
     </row>
-    <row r="355" spans="1:11">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>35011</v>
       </c>
@@ -12072,7 +12079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:11">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>35013</v>
       </c>
@@ -12098,7 +12105,7 @@
         <v>8.5085226999999999E-2</v>
       </c>
     </row>
-    <row r="357" spans="1:11">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>35015</v>
       </c>
@@ -12133,7 +12140,7 @@
         <v>2.460846E-3</v>
       </c>
     </row>
-    <row r="358" spans="1:11">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>35017</v>
       </c>
@@ -12168,7 +12175,7 @@
         <v>2.6492730000000002E-3</v>
       </c>
     </row>
-    <row r="359" spans="1:11">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>35019</v>
       </c>
@@ -12194,7 +12201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:11">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>35021</v>
       </c>
@@ -12214,7 +12221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:11">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>35023</v>
       </c>
@@ -12240,7 +12247,7 @@
         <v>5.1988635999999998E-2</v>
       </c>
     </row>
-    <row r="362" spans="1:11">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>35025</v>
       </c>
@@ -12275,7 +12282,7 @@
         <v>6.4565589999999997E-3</v>
       </c>
     </row>
-    <row r="363" spans="1:11">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>35027</v>
       </c>
@@ -12301,7 +12308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:11">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>35028</v>
       </c>
@@ -12321,7 +12328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:11">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>35029</v>
       </c>
@@ -12347,7 +12354,7 @@
         <v>7.8693182E-2</v>
       </c>
     </row>
-    <row r="366" spans="1:11">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>35031</v>
       </c>
@@ -12373,7 +12380,7 @@
         <v>0.13196022700000001</v>
       </c>
     </row>
-    <row r="367" spans="1:11">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>35033</v>
       </c>
@@ -12399,7 +12406,7 @@
         <v>5.8238636000000003E-2</v>
       </c>
     </row>
-    <row r="368" spans="1:11">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>35035</v>
       </c>
@@ -12425,7 +12432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:14">
+    <row r="369" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>35037</v>
       </c>
@@ -12451,7 +12458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:14">
+    <row r="370" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>35039</v>
       </c>
@@ -12477,7 +12484,7 @@
         <v>4.3465908999999997E-2</v>
       </c>
     </row>
-    <row r="371" spans="1:14">
+    <row r="371" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>35041</v>
       </c>
@@ -12503,7 +12510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:14">
+    <row r="372" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>35043</v>
       </c>
@@ -12529,7 +12536,7 @@
         <v>4.4318181999999998E-2</v>
       </c>
     </row>
-    <row r="373" spans="1:14">
+    <row r="373" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>35045</v>
       </c>
@@ -12549,7 +12556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:14">
+    <row r="374" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>35047</v>
       </c>
@@ -12575,7 +12582,7 @@
         <v>9.7301135999999996E-2</v>
       </c>
     </row>
-    <row r="375" spans="1:14">
+    <row r="375" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>35049</v>
       </c>
@@ -12610,7 +12617,7 @@
         <v>5.1093653000000003E-2</v>
       </c>
     </row>
-    <row r="376" spans="1:14">
+    <row r="376" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>35051</v>
       </c>
@@ -12636,7 +12643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:14">
+    <row r="377" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>35053</v>
       </c>
@@ -12662,7 +12669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:14">
+    <row r="378" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>35055</v>
       </c>
@@ -12682,7 +12689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:14">
+    <row r="379" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>35057</v>
       </c>
@@ -12708,7 +12715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:14">
+    <row r="380" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>35059</v>
       </c>
@@ -12734,7 +12741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:14">
+    <row r="381" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>35061</v>
       </c>
@@ -12760,7 +12767,7 @@
         <v>8.9062500000000003E-2</v>
       </c>
     </row>
-    <row r="382" spans="1:14">
+    <row r="382" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>41001</v>
       </c>
@@ -12792,7 +12799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:14">
+    <row r="383" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>41003</v>
       </c>
@@ -12824,7 +12831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:14">
+    <row r="384" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>41005</v>
       </c>
@@ -12856,7 +12863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:14">
+    <row r="385" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>41007</v>
       </c>
@@ -12891,7 +12898,7 @@
         <v>0.22033898299999999</v>
       </c>
     </row>
-    <row r="386" spans="1:14">
+    <row r="386" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>41009</v>
       </c>
@@ -12926,7 +12933,7 @@
         <v>5.0847457999999998E-2</v>
       </c>
     </row>
-    <row r="387" spans="1:14">
+    <row r="387" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>41011</v>
       </c>
@@ -12970,7 +12977,7 @@
         <v>6.7796609999999993E-2</v>
       </c>
     </row>
-    <row r="388" spans="1:14">
+    <row r="388" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>41013</v>
       </c>
@@ -13002,7 +13009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:14">
+    <row r="389" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>41015</v>
       </c>
@@ -13031,7 +13038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:14">
+    <row r="390" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>41017</v>
       </c>
@@ -13072,7 +13079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:14">
+    <row r="391" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>41019</v>
       </c>
@@ -13107,7 +13114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:14">
+    <row r="392" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>41021</v>
       </c>
@@ -13139,7 +13146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:14">
+    <row r="393" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>41023</v>
       </c>
@@ -13165,7 +13172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:14">
+    <row r="394" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>41025</v>
       </c>
@@ -13191,7 +13198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:14">
+    <row r="395" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>41027</v>
       </c>
@@ -13226,7 +13233,7 @@
         <v>3.3898304999999997E-2</v>
       </c>
     </row>
-    <row r="396" spans="1:14">
+    <row r="396" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>41029</v>
       </c>
@@ -13267,7 +13274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:14">
+    <row r="397" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>41031</v>
       </c>
@@ -13299,7 +13306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:14">
+    <row r="398" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>41033</v>
       </c>
@@ -13331,7 +13338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:14">
+    <row r="399" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>41035</v>
       </c>
@@ -13363,7 +13370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:14">
+    <row r="400" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>41037</v>
       </c>
@@ -13395,7 +13402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:14">
+    <row r="401" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>41039</v>
       </c>
@@ -13439,7 +13446,7 @@
         <v>1.6949153000000002E-2</v>
       </c>
     </row>
-    <row r="402" spans="1:14">
+    <row r="402" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>41041</v>
       </c>
@@ -13474,7 +13481,7 @@
         <v>3.3898304999999997E-2</v>
       </c>
     </row>
-    <row r="403" spans="1:14">
+    <row r="403" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>41043</v>
       </c>
@@ -13506,7 +13513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:14">
+    <row r="404" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A404">
         <v>41045</v>
       </c>
@@ -13538,7 +13545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:14">
+    <row r="405" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A405">
         <v>41047</v>
       </c>
@@ -13570,7 +13577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:14">
+    <row r="406" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>41049</v>
       </c>
@@ -13605,7 +13612,7 @@
         <v>1.6949153000000002E-2</v>
       </c>
     </row>
-    <row r="407" spans="1:14">
+    <row r="407" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>41051</v>
       </c>
@@ -13649,7 +13656,7 @@
         <v>0.52542372900000001</v>
       </c>
     </row>
-    <row r="408" spans="1:14">
+    <row r="408" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>41053</v>
       </c>
@@ -13681,7 +13688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:14">
+    <row r="409" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>41055</v>
       </c>
@@ -13713,7 +13720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:14">
+    <row r="410" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>41057</v>
       </c>
@@ -13748,7 +13755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:14">
+    <row r="411" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>41059</v>
       </c>
@@ -13792,7 +13799,7 @@
         <v>1.6949153000000002E-2</v>
       </c>
     </row>
-    <row r="412" spans="1:14">
+    <row r="412" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A412">
         <v>41061</v>
       </c>
@@ -13824,7 +13831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:14">
+    <row r="413" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A413">
         <v>41063</v>
       </c>
@@ -13856,7 +13863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:14">
+    <row r="414" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>41065</v>
       </c>
@@ -13891,7 +13898,7 @@
         <v>1.6949153000000002E-2</v>
       </c>
     </row>
-    <row r="415" spans="1:14">
+    <row r="415" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A415">
         <v>41067</v>
       </c>
@@ -13923,7 +13930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:14">
+    <row r="416" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A416">
         <v>41069</v>
       </c>
@@ -13949,7 +13956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:14">
+    <row r="417" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A417">
         <v>41071</v>
       </c>
@@ -13981,7 +13988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:14">
+    <row r="418" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A418">
         <v>49001</v>
       </c>
@@ -14007,7 +14014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:14">
+    <row r="419" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A419">
         <v>49003</v>
       </c>
@@ -14033,7 +14040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="420" spans="1:14">
+    <row r="420" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A420">
         <v>49005</v>
       </c>
@@ -14059,7 +14066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:14">
+    <row r="421" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A421">
         <v>49007</v>
       </c>
@@ -14085,7 +14092,7 @@
         <v>7.1277495999999996E-2</v>
       </c>
     </row>
-    <row r="422" spans="1:14">
+    <row r="422" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A422">
         <v>49009</v>
       </c>
@@ -14105,7 +14112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="423" spans="1:14">
+    <row r="423" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A423">
         <v>49011</v>
       </c>
@@ -14131,7 +14138,7 @@
         <v>5.4780033999999998E-2</v>
       </c>
     </row>
-    <row r="424" spans="1:14">
+    <row r="424" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A424">
         <v>49013</v>
       </c>
@@ -14151,7 +14158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:14">
+    <row r="425" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A425">
         <v>49015</v>
       </c>
@@ -14177,7 +14184,7 @@
         <v>0.116116751</v>
       </c>
     </row>
-    <row r="426" spans="1:14">
+    <row r="426" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A426">
         <v>49017</v>
       </c>
@@ -14197,7 +14204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="427" spans="1:14">
+    <row r="427" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A427">
         <v>49019</v>
       </c>
@@ -14232,7 +14239,7 @@
         <v>1.8037179999999999E-3</v>
       </c>
     </row>
-    <row r="428" spans="1:14">
+    <row r="428" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A428">
         <v>49021</v>
       </c>
@@ -14267,7 +14274,7 @@
         <v>1.149665E-3</v>
       </c>
     </row>
-    <row r="429" spans="1:14">
+    <row r="429" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A429">
         <v>49023</v>
       </c>
@@ -14293,7 +14300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="430" spans="1:14">
+    <row r="430" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A430">
         <v>49025</v>
       </c>
@@ -14313,7 +14320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="431" spans="1:14">
+    <row r="431" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A431">
         <v>49027</v>
       </c>
@@ -14339,7 +14346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="432" spans="1:14">
+    <row r="432" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A432">
         <v>49029</v>
       </c>
@@ -14365,7 +14372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="433" spans="1:14">
+    <row r="433" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A433">
         <v>49031</v>
       </c>
@@ -14385,7 +14392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="434" spans="1:14">
+    <row r="434" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>49033</v>
       </c>
@@ -14405,7 +14412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="435" spans="1:14">
+    <row r="435" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>49035</v>
       </c>
@@ -14440,7 +14447,7 @@
         <v>0.96913177100000003</v>
       </c>
     </row>
-    <row r="436" spans="1:14">
+    <row r="436" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>49037</v>
       </c>
@@ -14460,7 +14467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="437" spans="1:14">
+    <row r="437" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>49039</v>
       </c>
@@ -14480,7 +14487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="438" spans="1:14">
+    <row r="438" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A438">
         <v>49041</v>
       </c>
@@ -14500,7 +14507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="439" spans="1:14">
+    <row r="439" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A439">
         <v>49043</v>
       </c>
@@ -14526,7 +14533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="440" spans="1:14">
+    <row r="440" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>49045</v>
       </c>
@@ -14552,7 +14559,7 @@
         <v>0.21975465299999999</v>
       </c>
     </row>
-    <row r="441" spans="1:14">
+    <row r="441" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>49047</v>
       </c>
@@ -14587,7 +14594,7 @@
         <v>8.2299700000000001E-4</v>
       </c>
     </row>
-    <row r="442" spans="1:14">
+    <row r="442" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A442">
         <v>49049</v>
       </c>
@@ -14622,7 +14629,7 @@
         <v>1.0659106E-2</v>
       </c>
     </row>
-    <row r="443" spans="1:14">
+    <row r="443" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A443">
         <v>49051</v>
       </c>
@@ -14648,7 +14655,7 @@
         <v>3.7013536E-2</v>
       </c>
     </row>
-    <row r="444" spans="1:14">
+    <row r="444" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A444">
         <v>49053</v>
       </c>
@@ -14677,7 +14684,7 @@
         <v>1.3752527000000001E-2</v>
       </c>
     </row>
-    <row r="445" spans="1:14">
+    <row r="445" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A445">
         <v>49055</v>
       </c>
@@ -14697,7 +14704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="446" spans="1:14">
+    <row r="446" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A446">
         <v>49057</v>
       </c>
@@ -14732,7 +14739,7 @@
         <v>2.6802169999999999E-3</v>
       </c>
     </row>
-    <row r="447" spans="1:14">
+    <row r="447" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A447">
         <v>53001</v>
       </c>
@@ -14764,7 +14771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="448" spans="1:14">
+    <row r="448" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A448">
         <v>53003</v>
       </c>
@@ -14790,7 +14797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:14">
+    <row r="449" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A449">
         <v>53005</v>
       </c>
@@ -14825,7 +14832,7 @@
         <v>5.9523809999999996E-3</v>
       </c>
     </row>
-    <row r="450" spans="1:14">
+    <row r="450" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A450">
         <v>53007</v>
       </c>
@@ -14857,7 +14864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="451" spans="1:14">
+    <row r="451" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A451">
         <v>53009</v>
       </c>
@@ -14886,7 +14893,7 @@
         <v>8.9285714000000002E-2</v>
       </c>
     </row>
-    <row r="452" spans="1:14">
+    <row r="452" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A452">
         <v>53011</v>
       </c>
@@ -14921,7 +14928,7 @@
         <v>4.1666666999999998E-2</v>
       </c>
     </row>
-    <row r="453" spans="1:14">
+    <row r="453" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A453">
         <v>53013</v>
       </c>
@@ -14953,7 +14960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="454" spans="1:14">
+    <row r="454" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A454">
         <v>53015</v>
       </c>
@@ -14988,7 +14995,7 @@
         <v>1.7857142999999999E-2</v>
       </c>
     </row>
-    <row r="455" spans="1:14">
+    <row r="455" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A455">
         <v>53017</v>
       </c>
@@ -15029,7 +15036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="456" spans="1:14">
+    <row r="456" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A456">
         <v>53019</v>
       </c>
@@ -15061,7 +15068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="457" spans="1:14">
+    <row r="457" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A457">
         <v>53021</v>
       </c>
@@ -15105,7 +15112,7 @@
         <v>5.9523809999999996E-3</v>
       </c>
     </row>
-    <row r="458" spans="1:14">
+    <row r="458" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A458">
         <v>53023</v>
       </c>
@@ -15131,7 +15138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="459" spans="1:14">
+    <row r="459" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A459">
         <v>53025</v>
       </c>
@@ -15163,7 +15170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="460" spans="1:14">
+    <row r="460" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A460">
         <v>53027</v>
       </c>
@@ -15198,7 +15205,7 @@
         <v>2.9761905000000002E-2</v>
       </c>
     </row>
-    <row r="461" spans="1:14">
+    <row r="461" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A461">
         <v>53029</v>
       </c>
@@ -15227,7 +15234,7 @@
         <v>5.9523809999999996E-3</v>
       </c>
     </row>
-    <row r="462" spans="1:14">
+    <row r="462" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A462">
         <v>53031</v>
       </c>
@@ -15256,7 +15263,7 @@
         <v>2.9761905000000002E-2</v>
       </c>
     </row>
-    <row r="463" spans="1:14">
+    <row r="463" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A463">
         <v>53033</v>
       </c>
@@ -15300,7 +15307,7 @@
         <v>0.38095238100000001</v>
       </c>
     </row>
-    <row r="464" spans="1:14">
+    <row r="464" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A464">
         <v>53035</v>
       </c>
@@ -15335,7 +15342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="465" spans="1:14">
+    <row r="465" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A465">
         <v>53037</v>
       </c>
@@ -15367,7 +15374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="466" spans="1:14">
+    <row r="466" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A466">
         <v>53039</v>
       </c>
@@ -15402,7 +15409,7 @@
         <v>5.9523809999999996E-3</v>
       </c>
     </row>
-    <row r="467" spans="1:14">
+    <row r="467" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A467">
         <v>53041</v>
       </c>
@@ -15434,7 +15441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="468" spans="1:14">
+    <row r="468" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A468">
         <v>53043</v>
       </c>
@@ -15466,7 +15473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="469" spans="1:14">
+    <row r="469" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A469">
         <v>53045</v>
       </c>
@@ -15498,7 +15505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="470" spans="1:14">
+    <row r="470" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A470">
         <v>53047</v>
       </c>
@@ -15530,7 +15537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="471" spans="1:14">
+    <row r="471" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A471">
         <v>53049</v>
       </c>
@@ -15559,7 +15566,7 @@
         <v>1.1904761999999999E-2</v>
       </c>
     </row>
-    <row r="472" spans="1:14">
+    <row r="472" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A472">
         <v>53051</v>
       </c>
@@ -15591,7 +15598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="473" spans="1:14">
+    <row r="473" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A473">
         <v>53053</v>
       </c>
@@ -15626,7 +15633,7 @@
         <v>0.10714285699999999</v>
       </c>
     </row>
-    <row r="474" spans="1:14">
+    <row r="474" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A474">
         <v>53055</v>
       </c>
@@ -15661,7 +15668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="475" spans="1:14">
+    <row r="475" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A475">
         <v>53057</v>
       </c>
@@ -15696,7 +15703,7 @@
         <v>5.9523810000000003E-2</v>
       </c>
     </row>
-    <row r="476" spans="1:14">
+    <row r="476" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A476">
         <v>53059</v>
       </c>
@@ -15728,7 +15735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="477" spans="1:14">
+    <row r="477" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A477">
         <v>53061</v>
       </c>
@@ -15772,7 +15779,7 @@
         <v>8.3333332999999996E-2</v>
       </c>
     </row>
-    <row r="478" spans="1:14">
+    <row r="478" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A478">
         <v>53063</v>
       </c>
@@ -15813,7 +15820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="479" spans="1:14">
+    <row r="479" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A479">
         <v>53065</v>
       </c>
@@ -15845,7 +15852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="480" spans="1:14">
+    <row r="480" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A480">
         <v>53067</v>
       </c>
@@ -15880,7 +15887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="481" spans="1:14">
+    <row r="481" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A481">
         <v>53069</v>
       </c>
@@ -15909,7 +15916,7 @@
         <v>5.9523809999999996E-3</v>
       </c>
     </row>
-    <row r="482" spans="1:14">
+    <row r="482" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A482">
         <v>53071</v>
       </c>
@@ -15953,7 +15960,7 @@
         <v>1.1904761999999999E-2</v>
       </c>
     </row>
-    <row r="483" spans="1:14">
+    <row r="483" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A483">
         <v>53073</v>
       </c>
@@ -15997,7 +16004,7 @@
         <v>0.101190476</v>
       </c>
     </row>
-    <row r="484" spans="1:14">
+    <row r="484" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A484">
         <v>53075</v>
       </c>
@@ -16041,7 +16048,7 @@
         <v>5.9523809999999996E-3</v>
       </c>
     </row>
-    <row r="485" spans="1:14">
+    <row r="485" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A485">
         <v>53077</v>
       </c>
@@ -16082,7 +16089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="486" spans="1:14">
+    <row r="486" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A486">
         <v>56001</v>
       </c>
@@ -16117,7 +16124,7 @@
         <v>2.3810268999999998E-2</v>
       </c>
     </row>
-    <row r="487" spans="1:14">
+    <row r="487" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A487">
         <v>56003</v>
       </c>
@@ -16143,7 +16150,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="488" spans="1:14">
+    <row r="488" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A488">
         <v>56005</v>
       </c>
@@ -16178,7 +16185,7 @@
         <v>3.3980306000000002E-2</v>
       </c>
     </row>
-    <row r="489" spans="1:14">
+    <row r="489" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A489">
         <v>56007</v>
       </c>
@@ -16204,7 +16211,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="490" spans="1:14">
+    <row r="490" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A490">
         <v>56009</v>
       </c>
@@ -16230,7 +16237,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="491" spans="1:14">
+    <row r="491" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A491">
         <v>56011</v>
       </c>
@@ -16256,7 +16263,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="492" spans="1:14">
+    <row r="492" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A492">
         <v>56013</v>
       </c>
@@ -16291,7 +16298,7 @@
         <v>2.1948491000000001E-2</v>
       </c>
     </row>
-    <row r="493" spans="1:14">
+    <row r="493" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A493">
         <v>56015</v>
       </c>
@@ -16317,7 +16324,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="494" spans="1:14">
+    <row r="494" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A494">
         <v>56017</v>
       </c>
@@ -16343,7 +16350,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="495" spans="1:14">
+    <row r="495" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A495">
         <v>56019</v>
       </c>
@@ -16363,7 +16370,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="496" spans="1:14">
+    <row r="496" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A496">
         <v>56021</v>
       </c>
@@ -16398,7 +16405,7 @@
         <v>6.2742509999999998E-3</v>
       </c>
     </row>
-    <row r="497" spans="1:11">
+    <row r="497" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A497">
         <v>56023</v>
       </c>
@@ -16424,7 +16431,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="498" spans="1:11">
+    <row r="498" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A498">
         <v>56025</v>
       </c>
@@ -16459,7 +16466,7 @@
         <v>9.4838262000000007E-2</v>
       </c>
     </row>
-    <row r="499" spans="1:11">
+    <row r="499" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A499">
         <v>56027</v>
       </c>
@@ -16485,7 +16492,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="500" spans="1:11">
+    <row r="500" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A500">
         <v>56029</v>
       </c>
@@ -16520,7 +16527,7 @@
         <v>5.3161750000000001E-2</v>
       </c>
     </row>
-    <row r="501" spans="1:11">
+    <row r="501" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A501">
         <v>56031</v>
       </c>
@@ -16546,7 +16553,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="502" spans="1:11">
+    <row r="502" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A502">
         <v>56033</v>
       </c>
@@ -16581,7 +16588,7 @@
         <v>3.4047204999999997E-2</v>
       </c>
     </row>
-    <row r="503" spans="1:11">
+    <row r="503" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A503">
         <v>56035</v>
       </c>
@@ -16601,7 +16608,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="504" spans="1:11">
+    <row r="504" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A504">
         <v>56037</v>
       </c>
@@ -16636,7 +16643,7 @@
         <v>2.3740523999999999E-2</v>
       </c>
     </row>
-    <row r="505" spans="1:11">
+    <row r="505" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A505">
         <v>56039</v>
       </c>
@@ -16665,7 +16672,7 @@
         <v>0.70819894299999997</v>
       </c>
     </row>
-    <row r="506" spans="1:11">
+    <row r="506" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A506">
         <v>56041</v>
       </c>
@@ -16691,7 +16698,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="507" spans="1:11">
+    <row r="507" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A507">
         <v>56043</v>
       </c>
@@ -16717,7 +16724,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="508" spans="1:11">
+    <row r="508" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A508">
         <v>56045</v>
       </c>

</xml_diff>